<commit_message>
Update indexing of model names
</commit_message>
<xml_diff>
--- a/berts_of_a_feather/berts_of_a_feather_accuracies_by_run.xlsx
+++ b/berts_of_a_feather/berts_of_a_feather_accuracies_by_run.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommccoy/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96BA3994-04DC-6342-9251-42CE8BD7199B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A845CC4F-CCC3-864F-B6CF-0BDAFC6C7F43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="3620" windowWidth="28040" windowHeight="16240" xr2:uid="{731F26E3-8611-0E4F-A4A0-B0FB3CB89910}"/>
+    <workbookView xWindow="6120" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{731F26E3-8611-0E4F-A4A0-B0FB3CB89910}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="berts_of_a_feather_accuracies_b" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -441,9 +441,6 @@
     <t>Run 99</t>
   </si>
   <si>
-    <t>Run 100</t>
-  </si>
-  <si>
     <t>Minimum</t>
   </si>
   <si>
@@ -454,13 +451,16 @@
   </si>
   <si>
     <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Run 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,6 +480,12 @@
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -831,7 +837,7 @@
   <dimension ref="A1:AM112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AM105"/>
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -957,7 +963,7 @@
     </row>
     <row r="2" spans="1:39" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="B2" s="3">
         <v>0.84564439999999996</v>
@@ -1076,7 +1082,7 @@
     </row>
     <row r="3" spans="1:39" s="2" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3">
         <v>0.84360670000000004</v>
@@ -1195,7 +1201,7 @@
     </row>
     <row r="4" spans="1:39" s="2" customFormat="1">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3">
         <v>0.84768209999999999</v>
@@ -1314,7 +1320,7 @@
     </row>
     <row r="5" spans="1:39" s="2" customFormat="1">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3">
         <v>0.84279159999999997</v>
@@ -1433,7 +1439,7 @@
     </row>
     <row r="6" spans="1:39" s="2" customFormat="1">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3">
         <v>0.84268975000000002</v>
@@ -1552,7 +1558,7 @@
     </row>
     <row r="7" spans="1:39" s="2" customFormat="1">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3">
         <v>0.84248595999999998</v>
@@ -1671,7 +1677,7 @@
     </row>
     <row r="8" spans="1:39" s="2" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3">
         <v>0.8440143</v>
@@ -1790,7 +1796,7 @@
     </row>
     <row r="9" spans="1:39" s="2" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3">
         <v>0.84421800000000002</v>
@@ -1909,7 +1915,7 @@
     </row>
     <row r="10" spans="1:39" s="2" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3">
         <v>0.84421800000000002</v>
@@ -2028,7 +2034,7 @@
     </row>
     <row r="11" spans="1:39" s="2" customFormat="1">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3">
         <v>0.84564439999999996</v>
@@ -2147,7 +2153,7 @@
     </row>
     <row r="12" spans="1:39" s="2" customFormat="1">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="3">
         <v>0.84248595999999998</v>
@@ -2266,7 +2272,7 @@
     </row>
     <row r="13" spans="1:39" s="2" customFormat="1">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3">
         <v>0.84472745999999999</v>
@@ -2385,7 +2391,7 @@
     </row>
     <row r="14" spans="1:39" s="2" customFormat="1">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3">
         <v>0.84554255</v>
@@ -2504,7 +2510,7 @@
     </row>
     <row r="15" spans="1:39" s="2" customFormat="1">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3">
         <v>0.84574629999999995</v>
@@ -2623,7 +2629,7 @@
     </row>
     <row r="16" spans="1:39" s="2" customFormat="1">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3">
         <v>0.84513499999999997</v>
@@ -2742,7 +2748,7 @@
     </row>
     <row r="17" spans="1:39" s="2" customFormat="1">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3">
         <v>0.84095770000000003</v>
@@ -2861,7 +2867,7 @@
     </row>
     <row r="18" spans="1:39" s="2" customFormat="1">
       <c r="A18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="3">
         <v>0.84554255</v>
@@ -2980,7 +2986,7 @@
     </row>
     <row r="19" spans="1:39" s="2" customFormat="1">
       <c r="A19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="3">
         <v>0.84523689999999996</v>
@@ -3099,7 +3105,7 @@
     </row>
     <row r="20" spans="1:39" s="2" customFormat="1">
       <c r="A20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="3">
         <v>0.84085584000000002</v>
@@ -3218,7 +3224,7 @@
     </row>
     <row r="21" spans="1:39" s="2" customFormat="1">
       <c r="A21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="3">
         <v>0.84381050000000002</v>
@@ -3337,7 +3343,7 @@
     </row>
     <row r="22" spans="1:39" s="2" customFormat="1">
       <c r="A22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="3">
         <v>0.84177279999999999</v>
@@ -3456,7 +3462,7 @@
     </row>
     <row r="23" spans="1:39" s="2" customFormat="1">
       <c r="A23" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3">
         <v>0.84452366999999995</v>
@@ -3575,7 +3581,7 @@
     </row>
     <row r="24" spans="1:39" s="2" customFormat="1">
       <c r="A24" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="3">
         <v>0.84370862999999996</v>
@@ -3694,7 +3700,7 @@
     </row>
     <row r="25" spans="1:39" s="2" customFormat="1">
       <c r="A25" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="3">
         <v>0.84533875999999997</v>
@@ -3813,7 +3819,7 @@
     </row>
     <row r="26" spans="1:39" s="2" customFormat="1">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="3">
         <v>0.84462559999999998</v>
@@ -3932,7 +3938,7 @@
     </row>
     <row r="27" spans="1:39" s="2" customFormat="1">
       <c r="A27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="3">
         <v>0.84136529999999998</v>
@@ -4051,7 +4057,7 @@
     </row>
     <row r="28" spans="1:39" s="2" customFormat="1">
       <c r="A28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="3">
         <v>0.84207845000000003</v>
@@ -4170,7 +4176,7 @@
     </row>
     <row r="29" spans="1:39" s="2" customFormat="1">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="3">
         <v>0.8444218</v>
@@ -4289,7 +4295,7 @@
     </row>
     <row r="30" spans="1:39" s="2" customFormat="1">
       <c r="A30" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="3">
         <v>0.84207845000000003</v>
@@ -4408,7 +4414,7 @@
     </row>
     <row r="31" spans="1:39" s="2" customFormat="1">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="3">
         <v>0.84635764000000002</v>
@@ -4527,7 +4533,7 @@
     </row>
     <row r="32" spans="1:39" s="2" customFormat="1">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="3">
         <v>0.84564439999999996</v>
@@ -4646,7 +4652,7 @@
     </row>
     <row r="33" spans="1:39" s="2" customFormat="1">
       <c r="A33" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="3">
         <v>0.84299539999999995</v>
@@ -4765,7 +4771,7 @@
     </row>
     <row r="34" spans="1:39" s="2" customFormat="1">
       <c r="A34" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="3">
         <v>0.83912379999999998</v>
@@ -4884,7 +4890,7 @@
     </row>
     <row r="35" spans="1:39" s="2" customFormat="1">
       <c r="A35" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="3">
         <v>0.84105960000000002</v>
@@ -5003,7 +5009,7 @@
     </row>
     <row r="36" spans="1:39" s="2" customFormat="1">
       <c r="A36" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="3">
         <v>0.84462559999999998</v>
@@ -5122,7 +5128,7 @@
     </row>
     <row r="37" spans="1:39" s="2" customFormat="1">
       <c r="A37" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="3">
         <v>0.84350484999999997</v>
@@ -5241,7 +5247,7 @@
     </row>
     <row r="38" spans="1:39" s="2" customFormat="1">
       <c r="A38" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="3">
         <v>0.84146714</v>
@@ -5360,7 +5366,7 @@
     </row>
     <row r="39" spans="1:39" s="2" customFormat="1">
       <c r="A39" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39" s="3">
         <v>0.84411614999999995</v>
@@ -5479,7 +5485,7 @@
     </row>
     <row r="40" spans="1:39" s="2" customFormat="1">
       <c r="A40" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40" s="3">
         <v>0.84309730000000005</v>
@@ -5598,7 +5604,7 @@
     </row>
     <row r="41" spans="1:39" s="2" customFormat="1">
       <c r="A41" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41" s="3">
         <v>0.84350484999999997</v>
@@ -5717,7 +5723,7 @@
     </row>
     <row r="42" spans="1:39" s="2" customFormat="1">
       <c r="A42" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" s="3">
         <v>0.8440143</v>
@@ -5836,7 +5842,7 @@
     </row>
     <row r="43" spans="1:39" s="2" customFormat="1">
       <c r="A43" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="3">
         <v>0.84136529999999998</v>
@@ -5955,7 +5961,7 @@
     </row>
     <row r="44" spans="1:39" s="2" customFormat="1">
       <c r="A44" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" s="3">
         <v>0.83942943999999997</v>
@@ -6074,7 +6080,7 @@
     </row>
     <row r="45" spans="1:39" s="2" customFormat="1">
       <c r="A45" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="3">
         <v>0.84411614999999995</v>
@@ -6193,7 +6199,7 @@
     </row>
     <row r="46" spans="1:39" s="2" customFormat="1">
       <c r="A46" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B46" s="3">
         <v>0.83667855999999996</v>
@@ -6312,7 +6318,7 @@
     </row>
     <row r="47" spans="1:39" s="2" customFormat="1">
       <c r="A47" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="3">
         <v>0.84309730000000005</v>
@@ -6431,7 +6437,7 @@
     </row>
     <row r="48" spans="1:39" s="2" customFormat="1">
       <c r="A48" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="3">
         <v>0.84055020000000003</v>
@@ -6550,7 +6556,7 @@
     </row>
     <row r="49" spans="1:39" s="2" customFormat="1">
       <c r="A49" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="3">
         <v>0.84676516000000002</v>
@@ -6669,7 +6675,7 @@
     </row>
     <row r="50" spans="1:39" s="2" customFormat="1">
       <c r="A50" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="3">
         <v>0.84034640000000005</v>
@@ -6788,7 +6794,7 @@
     </row>
     <row r="51" spans="1:39" s="2" customFormat="1">
       <c r="A51" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" s="3">
         <v>0.84635764000000002</v>
@@ -6907,7 +6913,7 @@
     </row>
     <row r="52" spans="1:39" s="2" customFormat="1">
       <c r="A52" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B52" s="3">
         <v>0.84513499999999997</v>
@@ -7026,7 +7032,7 @@
     </row>
     <row r="53" spans="1:39" s="2" customFormat="1">
       <c r="A53" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" s="3">
         <v>0.84656140000000002</v>
@@ -7145,7 +7151,7 @@
     </row>
     <row r="54" spans="1:39" s="2" customFormat="1">
       <c r="A54" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B54" s="3">
         <v>0.83932759999999995</v>
@@ -7264,7 +7270,7 @@
     </row>
     <row r="55" spans="1:39" s="2" customFormat="1">
       <c r="A55" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B55" s="3">
         <v>0.84299539999999995</v>
@@ -7383,7 +7389,7 @@
     </row>
     <row r="56" spans="1:39" s="2" customFormat="1">
       <c r="A56" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B56" s="3">
         <v>0.84370862999999996</v>
@@ -7502,7 +7508,7 @@
     </row>
     <row r="57" spans="1:39" s="2" customFormat="1">
       <c r="A57" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B57" s="3">
         <v>0.84482930000000001</v>
@@ -7621,7 +7627,7 @@
     </row>
     <row r="58" spans="1:39" s="2" customFormat="1">
       <c r="A58" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B58" s="3">
         <v>0.83892</v>
@@ -7740,7 +7746,7 @@
     </row>
     <row r="59" spans="1:39" s="2" customFormat="1">
       <c r="A59" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B59" s="3">
         <v>0.84319920000000004</v>
@@ -7859,7 +7865,7 @@
     </row>
     <row r="60" spans="1:39" s="2" customFormat="1">
       <c r="A60" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B60" s="3">
         <v>0.84218029999999999</v>
@@ -7978,7 +7984,7 @@
     </row>
     <row r="61" spans="1:39" s="2" customFormat="1">
       <c r="A61" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B61" s="3">
         <v>0.84707080000000001</v>
@@ -8097,7 +8103,7 @@
     </row>
     <row r="62" spans="1:39" s="2" customFormat="1">
       <c r="A62" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B62" s="3">
         <v>0.84452366999999995</v>
@@ -8216,7 +8222,7 @@
     </row>
     <row r="63" spans="1:39" s="2" customFormat="1">
       <c r="A63" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B63" s="3">
         <v>0.83993890000000004</v>
@@ -8335,7 +8341,7 @@
     </row>
     <row r="64" spans="1:39" s="2" customFormat="1">
       <c r="A64" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B64" s="3">
         <v>0.84431993999999999</v>
@@ -8454,7 +8460,7 @@
     </row>
     <row r="65" spans="1:39" s="2" customFormat="1">
       <c r="A65" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B65" s="3">
         <v>0.83881813000000005</v>
@@ -8573,7 +8579,7 @@
     </row>
     <row r="66" spans="1:39" s="2" customFormat="1">
       <c r="A66" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B66" s="3">
         <v>0.84686700000000004</v>
@@ -8692,7 +8698,7 @@
     </row>
     <row r="67" spans="1:39" s="2" customFormat="1">
       <c r="A67" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B67" s="3">
         <v>0.84656140000000002</v>
@@ -8811,7 +8817,7 @@
     </row>
     <row r="68" spans="1:39" s="2" customFormat="1">
       <c r="A68" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B68" s="3">
         <v>0.84482930000000001</v>
@@ -8930,7 +8936,7 @@
     </row>
     <row r="69" spans="1:39" s="2" customFormat="1">
       <c r="A69" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B69" s="3">
         <v>0.84238409999999997</v>
@@ -9049,7 +9055,7 @@
     </row>
     <row r="70" spans="1:39" s="2" customFormat="1">
       <c r="A70" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B70" s="3">
         <v>0.84635764000000002</v>
@@ -9168,7 +9174,7 @@
     </row>
     <row r="71" spans="1:39" s="2" customFormat="1">
       <c r="A71" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B71" s="3">
         <v>0.84248595999999998</v>
@@ -9287,7 +9293,7 @@
     </row>
     <row r="72" spans="1:39" s="2" customFormat="1">
       <c r="A72" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B72" s="3">
         <v>0.83851249999999999</v>
@@ -9406,7 +9412,7 @@
     </row>
     <row r="73" spans="1:39" s="2" customFormat="1">
       <c r="A73" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B73" s="3">
         <v>0.84105960000000002</v>
@@ -9525,7 +9531,7 @@
     </row>
     <row r="74" spans="1:39" s="2" customFormat="1">
       <c r="A74" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B74" s="3">
         <v>0.84411614999999995</v>
@@ -9644,7 +9650,7 @@
     </row>
     <row r="75" spans="1:39" s="2" customFormat="1">
       <c r="A75" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B75" s="3">
         <v>0.83678039999999998</v>
@@ -9763,7 +9769,7 @@
     </row>
     <row r="76" spans="1:39" s="2" customFormat="1">
       <c r="A76" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B76" s="3">
         <v>0.8444218</v>
@@ -9882,7 +9888,7 @@
     </row>
     <row r="77" spans="1:39" s="2" customFormat="1">
       <c r="A77" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B77" s="3">
         <v>0.84381050000000002</v>
@@ -10001,7 +10007,7 @@
     </row>
     <row r="78" spans="1:39" s="2" customFormat="1">
       <c r="A78" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B78" s="3">
         <v>0.83922565000000005</v>
@@ -10120,7 +10126,7 @@
     </row>
     <row r="79" spans="1:39" s="2" customFormat="1">
       <c r="A79" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B79" s="3">
         <v>0.84330099999999997</v>
@@ -10239,7 +10245,7 @@
     </row>
     <row r="80" spans="1:39" s="2" customFormat="1">
       <c r="A80" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B80" s="3">
         <v>0.84523689999999996</v>
@@ -10358,7 +10364,7 @@
     </row>
     <row r="81" spans="1:39" s="2" customFormat="1">
       <c r="A81" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B81" s="3">
         <v>0.8440143</v>
@@ -10477,7 +10483,7 @@
     </row>
     <row r="82" spans="1:39" s="2" customFormat="1">
       <c r="A82" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B82" s="3">
         <v>0.84533875999999997</v>
@@ -10596,7 +10602,7 @@
     </row>
     <row r="83" spans="1:39" s="2" customFormat="1">
       <c r="A83" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B83" s="3">
         <v>0.84472745999999999</v>
@@ -10715,7 +10721,7 @@
     </row>
     <row r="84" spans="1:39" s="2" customFormat="1">
       <c r="A84" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B84" s="3">
         <v>0.84462559999999998</v>
@@ -10834,7 +10840,7 @@
     </row>
     <row r="85" spans="1:39" s="2" customFormat="1">
       <c r="A85" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B85" s="3">
         <v>0.84493123999999997</v>
@@ -10953,7 +10959,7 @@
     </row>
     <row r="86" spans="1:39" s="2" customFormat="1">
       <c r="A86" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B86" s="3">
         <v>0.84381050000000002</v>
@@ -11072,7 +11078,7 @@
     </row>
     <row r="87" spans="1:39" s="2" customFormat="1">
       <c r="A87" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B87" s="3">
         <v>0.84645950000000003</v>
@@ -11191,7 +11197,7 @@
     </row>
     <row r="88" spans="1:39" s="2" customFormat="1">
       <c r="A88" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B88" s="3">
         <v>0.84370862999999996</v>
@@ -11310,7 +11316,7 @@
     </row>
     <row r="89" spans="1:39" s="2" customFormat="1">
       <c r="A89" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B89" s="3">
         <v>0.84411614999999995</v>
@@ -11429,7 +11435,7 @@
     </row>
     <row r="90" spans="1:39" s="2" customFormat="1">
       <c r="A90" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B90" s="3">
         <v>0.84197659999999996</v>
@@ -11548,7 +11554,7 @@
     </row>
     <row r="91" spans="1:39" s="2" customFormat="1">
       <c r="A91" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B91" s="3">
         <v>0.83739173</v>
@@ -11667,7 +11673,7 @@
     </row>
     <row r="92" spans="1:39" s="2" customFormat="1">
       <c r="A92" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B92" s="3">
         <v>0.84218029999999999</v>
@@ -11786,7 +11792,7 @@
     </row>
     <row r="93" spans="1:39" s="2" customFormat="1">
       <c r="A93" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B93" s="3">
         <v>0.84513499999999997</v>
@@ -11905,7 +11911,7 @@
     </row>
     <row r="94" spans="1:39" s="2" customFormat="1">
       <c r="A94" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B94" s="3">
         <v>0.84595007</v>
@@ -12024,7 +12030,7 @@
     </row>
     <row r="95" spans="1:39" s="2" customFormat="1">
       <c r="A95" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B95" s="3">
         <v>0.84452366999999995</v>
@@ -12143,7 +12149,7 @@
     </row>
     <row r="96" spans="1:39" s="2" customFormat="1">
       <c r="A96" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B96" s="3">
         <v>0.84279159999999997</v>
@@ -12262,7 +12268,7 @@
     </row>
     <row r="97" spans="1:39" s="2" customFormat="1">
       <c r="A97" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B97" s="3">
         <v>0.84645950000000003</v>
@@ -12381,7 +12387,7 @@
     </row>
     <row r="98" spans="1:39" s="2" customFormat="1">
       <c r="A98" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B98" s="3">
         <v>0.84350484999999997</v>
@@ -12500,7 +12506,7 @@
     </row>
     <row r="99" spans="1:39" s="2" customFormat="1">
       <c r="A99" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B99" s="3">
         <v>0.84014266999999998</v>
@@ -12619,7 +12625,7 @@
     </row>
     <row r="100" spans="1:39" s="2" customFormat="1">
       <c r="A100" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B100" s="3">
         <v>0.84768209999999999</v>
@@ -12738,7 +12744,7 @@
     </row>
     <row r="101" spans="1:39" s="2" customFormat="1">
       <c r="A101" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B101" s="3">
         <v>0.84116150000000001</v>
@@ -12857,7 +12863,7 @@
     </row>
     <row r="102" spans="1:39">
       <c r="A102" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B102" s="4">
         <f xml:space="preserve"> MIN(B2:B101)</f>
@@ -13014,7 +13020,7 @@
     </row>
     <row r="103" spans="1:39">
       <c r="A103" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B103" s="4">
         <f xml:space="preserve"> MAX(B2:B101)</f>
@@ -13171,7 +13177,7 @@
     </row>
     <row r="104" spans="1:39">
       <c r="A104" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B104" s="4">
         <f xml:space="preserve"> AVERAGE(B2:B101)</f>
@@ -13328,7 +13334,7 @@
     </row>
     <row r="105" spans="1:39">
       <c r="A105" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B105" s="4">
         <f xml:space="preserve"> STDEV(B2:B101)</f>
@@ -13487,6 +13493,7 @@
       <c r="B112" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>